<commit_message>
Starting the trust model
</commit_message>
<xml_diff>
--- a/Cross-Validation SVM/SupportVextors/ResultMat/AndreiData & Other Users Test Data.xlsx
+++ b/Cross-Validation SVM/SupportVextors/ResultMat/AndreiData & Other Users Test Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="andrei - flag 1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'andrei - flag 1'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Carolina</t>
   </si>
@@ -59,6 +59,33 @@
   </si>
   <si>
     <t>Bianca Lazar</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Confidence Start</t>
+  </si>
+  <si>
+    <t>Sum 3 Obs</t>
+  </si>
+  <si>
+    <t>Sum 5 Obs</t>
+  </si>
+  <si>
+    <t>Sum 7 Obs</t>
+  </si>
+  <si>
+    <t>Sum 10 obs</t>
+  </si>
+  <si>
+    <t>Sum 12 Obs</t>
+  </si>
+  <si>
+    <t>Sum 15 Obs</t>
+  </si>
+  <si>
+    <t>Confidence Changes</t>
   </si>
 </sst>
 </file>
@@ -382,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -532,6 +559,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -577,11 +673,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -905,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,16 +4100,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ES12"/>
+  <dimension ref="A1:ES17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:149" x14ac:dyDescent="0.25">
@@ -6884,6 +6994,94 @@
         <v>4.3911284999999998</v>
       </c>
     </row>
+    <row r="15" spans="1:149" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:149" x14ac:dyDescent="0.25">
+      <c r="C16" s="7">
+        <v>80</v>
+      </c>
+      <c r="D16" s="8">
+        <v>100</v>
+      </c>
+      <c r="E16" s="8">
+        <f>SUM(B2:D2)</f>
+        <v>6.6601185999999997</v>
+      </c>
+      <c r="F16" s="8">
+        <f>SUM(B2:F2)</f>
+        <v>12.000944799999999</v>
+      </c>
+      <c r="G16" s="8">
+        <f>SUM(B2:H2)</f>
+        <v>18.343036099999999</v>
+      </c>
+      <c r="H16" s="8">
+        <f>SUM(B2:K2)</f>
+        <v>27.100233800000002</v>
+      </c>
+      <c r="I16" s="8">
+        <f>SUM(B2:M2)</f>
+        <v>35.701065200000002</v>
+      </c>
+      <c r="J16" s="9">
+        <f>SUM(B2:P2)</f>
+        <v>45.424616</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+      <c r="D17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="11">
+        <f>SUM(D16, -E16)</f>
+        <v>93.339881399999996</v>
+      </c>
+      <c r="F17" s="11">
+        <f>SUM(D16, -F16)</f>
+        <v>87.999055200000001</v>
+      </c>
+      <c r="G17" s="11">
+        <f>SUM(D16, -G16)</f>
+        <v>81.656963899999994</v>
+      </c>
+      <c r="H17" s="11">
+        <f>SUM(D16, -H16)</f>
+        <v>72.899766200000002</v>
+      </c>
+      <c r="I17" s="11">
+        <f>SUM(D16, -I16)</f>
+        <v>64.298934799999998</v>
+      </c>
+      <c r="J17" s="1">
+        <f>SUM(D16, -J16)</f>
+        <v>54.575384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>